<commit_message>
iniciando as analises dos dados
</commit_message>
<xml_diff>
--- a/Aula_29_02_2024_ANOVA/notas_precos.xlsx
+++ b/Aula_29_02_2024_ANOVA/notas_precos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\asn_exercicios\Aula_29_02_2024_ANOVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EE00A5-29E0-44EA-ADF5-592C24C93C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8388E632-4CA9-414A-AD4D-77EBE2C19666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE2A588F-1152-4563-9171-2B5D313C0575}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE2A588F-1152-4563-9171-2B5D313C0575}"/>
   </bookViews>
   <sheets>
     <sheet name="preco_nota" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -139,6 +143,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68DFBEA5-3892-4473-842C-43187B6CDBC1}" name="Table2" displayName="Table2" ref="A1:B61" totalsRowShown="0">
+  <autoFilter ref="A1:B61" xr:uid="{68DFBEA5-3892-4473-842C-43187B6CDBC1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{24DA6E05-D72D-46CC-A69F-5B618BF4E184}" name="faixa_preco"/>
+    <tableColumn id="2" xr3:uid="{ADF4FF32-9FA0-4AC4-BAEF-91591155D2B1}" name="notas" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,13 +475,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A5063F-51DD-4437-8776-CD4CC063B9A2}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -961,6 +976,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -968,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76E8E00-AA1B-4E16-A3F9-D7F514744314}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>